<commit_message>
Adds additional submission forms, improves and add logic for processing forms. Currently all forms are being created, but not fully filled yet.
</commit_message>
<xml_diff>
--- a/requests/ECHO_HIV_HI_PBMC_csrna-seq.xlsx
+++ b/requests/ECHO_HIV_HI_PBMC_csrna-seq.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MounSinai\Darpa\Programming\submission\requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCD5DA7-FD95-4DA9-9921-86C1DE55F4BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B7D7E33-664B-4DDC-BA8A-87354FBA7A12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11265" xr2:uid="{1022EA94-C927-47D4-994A-3445E7764CD5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1022EA94-C927-47D4-994A-3445E7764CD5}"/>
   </bookViews>
   <sheets>
     <sheet name="Submission_Request" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="67">
   <si>
     <t>Project</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Sub-Aliquots</t>
   </si>
   <si>
-    <t>Aliquots (optional)</t>
-  </si>
-  <si>
     <t>HIV</t>
   </si>
   <si>
@@ -223,6 +220,18 @@
   </si>
   <si>
     <t>AS09-13278</t>
+  </si>
+  <si>
+    <t>Sample_id</t>
+  </si>
+  <si>
+    <t>Experiment_id</t>
+  </si>
+  <si>
+    <t>Exp_123</t>
+  </si>
+  <si>
+    <t>AS17-00144</t>
   </si>
 </sst>
 </file>
@@ -592,7 +601,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{648F6FB2-DCD5-4DC2-9468-8A496EE9201E}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
@@ -604,9 +613,10 @@
     <col min="5" max="5" width="10.28515625" customWidth="1"/>
     <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -626,46 +636,55 @@
         <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" t="s">
         <v>58</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F3" t="s">
+      <c r="G3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
         <v>60</v>
       </c>
-      <c r="G3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>61</v>
       </c>
-      <c r="G4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G5" s="1"/>
     </row>
   </sheetData>
@@ -710,103 +729,103 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -814,110 +833,110 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>